<commit_message>
Add float type item to GEM
</commit_message>
<xml_diff>
--- a/documentation/Menu.xlsx
+++ b/documentation/Menu.xlsx
@@ -8,17 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_SOURCE_SOFT\MiniThread\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD383CF-84E0-40DC-9DE3-28E160A970E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA18C926-66DB-4CB2-984E-B8AB55111D95}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -527,7 +533,7 @@
   <dimension ref="A2:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Ajout changement écran avec OK
</commit_message>
<xml_diff>
--- a/documentation/Menu.xlsx
+++ b/documentation/Menu.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_SOURCE_SOFT\MiniThread\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10A7183-52C1-47BA-9936-D020EDD3D679}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA47573-956A-40D1-B0A3-CC92716FCAFB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Menu" sheetId="1" r:id="rId1"/>
+    <sheet name="Navigation" sheetId="2" r:id="rId1"/>
+    <sheet name="Menu" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>UseMotor</t>
   </si>
@@ -81,22 +79,10 @@
     <t>Thread</t>
   </si>
   <si>
-    <t>Start the mode</t>
-  </si>
-  <si>
-    <t>button</t>
-  </si>
-  <si>
-    <t>Stop the mode</t>
-  </si>
-  <si>
     <t>Speed of the motor during Manual mode and return during threading</t>
   </si>
   <si>
     <t>Example</t>
-  </si>
-  <si>
-    <t>True</t>
   </si>
   <si>
     <t>Manual</t>
@@ -165,13 +151,49 @@
   </si>
   <si>
     <t>fMotorCurrentPos</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Cancel / Menu</t>
+  </si>
+  <si>
+    <t>Boutons de navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -10.23</t>
+  </si>
+  <si>
+    <t>24.3</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Menu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,8 +209,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,8 +240,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -247,28 +307,180 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,259 +760,448 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7A3DD7-84B1-4623-A087-5B67F1819918}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="4.44140625" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" customWidth="1"/>
+    <col min="4" max="4" width="2.77734375" customWidth="1"/>
+    <col min="5" max="5" width="7.77734375" customWidth="1"/>
+    <col min="6" max="6" width="2.77734375" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" customWidth="1"/>
+    <col min="8" max="8" width="1.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="4.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="1:10" ht="7.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="1:10" ht="7.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="6" width="13.44140625" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="19"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D10" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="C11" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="5">
-        <v>-10</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="5">
+      <c r="E11" s="1">
         <v>100</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="5">
-        <v>2</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="5">
-        <v>100</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="2"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>